<commit_message>
getEvents -- if org is null
</commit_message>
<xml_diff>
--- a/jan7to21v3.xlsx
+++ b/jan7to21v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6060" yWindow="460" windowWidth="28560" windowHeight="16560"/>
+    <workbookView xWindow="200" yWindow="740" windowWidth="28560" windowHeight="16560"/>
   </bookViews>
   <sheets>
     <sheet name="bbsk8r1@gmail.com" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>